<commit_message>
finishing chauvenet and finishing dcos 2.1
</commit_message>
<xml_diff>
--- a/Arduino-Bluetooth/docs 2nd Approach/tukey_hsd.xlsx
+++ b/Arduino-Bluetooth/docs 2nd Approach/tukey_hsd.xlsx
@@ -503,7 +503,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Rejected</t>
         </is>
       </c>
     </row>
@@ -535,7 +535,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>Accepted</t>
         </is>
       </c>
     </row>
@@ -567,7 +567,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>Accepted</t>
         </is>
       </c>
     </row>
@@ -599,7 +599,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>Accepted</t>
         </is>
       </c>
     </row>
@@ -631,7 +631,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>Accepted</t>
         </is>
       </c>
     </row>
@@ -663,7 +663,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Rejected</t>
         </is>
       </c>
     </row>
@@ -695,7 +695,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Rejected</t>
         </is>
       </c>
     </row>
@@ -727,7 +727,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Rejected</t>
         </is>
       </c>
     </row>
@@ -759,7 +759,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Rejected</t>
         </is>
       </c>
     </row>
@@ -791,7 +791,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Rejected</t>
         </is>
       </c>
     </row>
@@ -823,7 +823,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Rejected</t>
         </is>
       </c>
     </row>
@@ -855,7 +855,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Rejected</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Rejected</t>
         </is>
       </c>
     </row>
@@ -919,7 +919,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Rejected</t>
         </is>
       </c>
     </row>
@@ -951,7 +951,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Rejected</t>
         </is>
       </c>
     </row>
@@ -983,7 +983,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>Accepted</t>
         </is>
       </c>
     </row>
@@ -1015,7 +1015,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>Accepted</t>
         </is>
       </c>
     </row>
@@ -1047,7 +1047,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Rejected</t>
         </is>
       </c>
     </row>
@@ -1079,7 +1079,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Rejected</t>
         </is>
       </c>
     </row>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Rejected</t>
         </is>
       </c>
     </row>
@@ -1143,7 +1143,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Rejected</t>
         </is>
       </c>
     </row>
@@ -1175,7 +1175,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>Accepted</t>
         </is>
       </c>
     </row>
@@ -1207,7 +1207,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Rejected</t>
         </is>
       </c>
     </row>
@@ -1239,7 +1239,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Rejected</t>
         </is>
       </c>
     </row>
@@ -1271,7 +1271,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Rejected</t>
         </is>
       </c>
     </row>
@@ -1303,7 +1303,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Rejected</t>
         </is>
       </c>
     </row>
@@ -1335,7 +1335,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>Accepted</t>
         </is>
       </c>
     </row>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Rejected</t>
         </is>
       </c>
     </row>
@@ -1399,7 +1399,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Rejected</t>
         </is>
       </c>
     </row>
@@ -1431,7 +1431,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Rejected</t>
         </is>
       </c>
     </row>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Rejected</t>
         </is>
       </c>
     </row>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Rejected</t>
         </is>
       </c>
     </row>
@@ -1527,7 +1527,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Rejected</t>
         </is>
       </c>
     </row>
@@ -1559,7 +1559,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>Accepted</t>
         </is>
       </c>
     </row>
@@ -1591,7 +1591,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Rejected</t>
         </is>
       </c>
     </row>
@@ -1623,7 +1623,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Rejected</t>
         </is>
       </c>
     </row>

</xml_diff>